<commit_message>
Add neutro maturity gene set
</commit_message>
<xml_diff>
--- a/tables/gene_annotations/neutro_phenotype_genesets.xlsx
+++ b/tables/gene_annotations/neutro_phenotype_genesets.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="417">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1049,6 +1049,24 @@
   </si>
   <si>
     <t xml:space="preserve">MIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mature_immature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCRL2</t>
   </si>
   <si>
     <t xml:space="preserve">Gene name</t>
@@ -1593,12 +1611,12 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B123" activeCellId="0" sqref="B123"/>
+      <selection pane="bottomLeft" activeCell="C281" activeCellId="0" sqref="C281"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.1328125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.67"/>
@@ -3007,7 +3025,7 @@
       <c r="B125" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E125" s="0" t="s">
+      <c r="E125" s="3" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3034,7 +3052,7 @@
       <c r="B128" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E128" s="0" t="s">
+      <c r="E128" s="3" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3109,7 +3127,7 @@
       <c r="A137" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B137" s="0" t="s">
+      <c r="B137" s="3" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3117,7 +3135,7 @@
       <c r="A138" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B138" s="0" t="s">
+      <c r="B138" s="3" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3125,7 +3143,7 @@
       <c r="A139" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B139" s="0" t="s">
+      <c r="B139" s="3" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3133,7 +3151,7 @@
       <c r="A140" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B140" s="0" t="s">
+      <c r="B140" s="3" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3141,7 +3159,7 @@
       <c r="A141" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B141" s="0" t="s">
+      <c r="B141" s="3" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3149,7 +3167,7 @@
       <c r="A142" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B142" s="0" t="s">
+      <c r="B142" s="3" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3157,7 +3175,7 @@
       <c r="A143" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B143" s="0" t="s">
+      <c r="B143" s="3" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3165,7 +3183,7 @@
       <c r="A144" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B144" s="0" t="s">
+      <c r="B144" s="3" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3173,7 +3191,7 @@
       <c r="A145" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B145" s="0" t="s">
+      <c r="B145" s="3" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3181,7 +3199,7 @@
       <c r="A146" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B146" s="0" t="s">
+      <c r="B146" s="3" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3189,7 +3207,7 @@
       <c r="A147" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B147" s="0" t="s">
+      <c r="B147" s="3" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3197,7 +3215,7 @@
       <c r="A148" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B148" s="0" t="s">
+      <c r="B148" s="3" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3205,7 +3223,7 @@
       <c r="A149" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B149" s="0" t="s">
+      <c r="B149" s="3" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3213,7 +3231,7 @@
       <c r="A150" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B150" s="0" t="s">
+      <c r="B150" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3221,7 +3239,7 @@
       <c r="A151" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B151" s="0" t="s">
+      <c r="B151" s="3" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3229,7 +3247,7 @@
       <c r="A152" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B152" s="0" t="s">
+      <c r="B152" s="3" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3237,7 +3255,7 @@
       <c r="A153" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B153" s="0" t="s">
+      <c r="B153" s="3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3245,7 +3263,7 @@
       <c r="A154" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="B154" s="3" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3253,7 +3271,7 @@
       <c r="A155" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B155" s="0" t="s">
+      <c r="B155" s="3" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3261,7 +3279,7 @@
       <c r="A156" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B156" s="0" t="s">
+      <c r="B156" s="3" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3269,7 +3287,7 @@
       <c r="A157" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="B157" s="3" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3277,7 +3295,7 @@
       <c r="A158" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B158" s="0" t="s">
+      <c r="B158" s="3" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3285,7 +3303,7 @@
       <c r="A159" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B159" s="0" t="s">
+      <c r="B159" s="3" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3293,7 +3311,7 @@
       <c r="A160" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B160" s="0" t="s">
+      <c r="B160" s="3" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4132,7 +4150,7 @@
       <c r="A263" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B263" s="0" t="s">
+      <c r="B263" s="3" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4140,7 +4158,7 @@
       <c r="A264" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B264" s="0" t="s">
+      <c r="B264" s="3" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4148,7 +4166,7 @@
       <c r="A265" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B265" s="0" t="s">
+      <c r="B265" s="3" t="s">
         <v>258</v>
       </c>
     </row>
@@ -4156,7 +4174,7 @@
       <c r="A266" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B266" s="0" t="s">
+      <c r="B266" s="3" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4164,7 +4182,7 @@
       <c r="A267" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B267" s="0" t="s">
+      <c r="B267" s="3" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4172,7 +4190,7 @@
       <c r="A268" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B268" s="0" t="s">
+      <c r="B268" s="3" t="s">
         <v>319</v>
       </c>
     </row>
@@ -4180,7 +4198,7 @@
       <c r="A269" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B269" s="0" t="s">
+      <c r="B269" s="3" t="s">
         <v>320</v>
       </c>
     </row>
@@ -4188,7 +4206,7 @@
       <c r="A270" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B270" s="0" t="s">
+      <c r="B270" s="3" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4196,7 +4214,7 @@
       <c r="A271" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B271" s="0" t="s">
+      <c r="B271" s="3" t="s">
         <v>251</v>
       </c>
     </row>
@@ -4204,7 +4222,7 @@
       <c r="A272" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B272" s="0" t="s">
+      <c r="B272" s="3" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4212,7 +4230,7 @@
       <c r="A273" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B273" s="0" t="s">
+      <c r="B273" s="3" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4220,7 +4238,7 @@
       <c r="A274" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B274" s="0" t="s">
+      <c r="B274" s="3" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4228,7 +4246,7 @@
       <c r="A275" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B275" s="0" t="s">
+      <c r="B275" s="3" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4236,7 +4254,7 @@
       <c r="A276" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B276" s="0" t="s">
+      <c r="B276" s="3" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4244,7 +4262,7 @@
       <c r="A277" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B277" s="0" t="s">
+      <c r="B277" s="3" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4252,7 +4270,7 @@
       <c r="A278" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B278" s="0" t="s">
+      <c r="B278" s="3" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4260,7 +4278,7 @@
       <c r="A279" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B279" s="0" t="s">
+      <c r="B279" s="3" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4268,7 +4286,7 @@
       <c r="A280" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B280" s="0" t="s">
+      <c r="B280" s="3" t="s">
         <v>329</v>
       </c>
     </row>
@@ -4276,7 +4294,7 @@
       <c r="A281" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B281" s="0" t="s">
+      <c r="B281" s="3" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4284,7 +4302,7 @@
       <c r="A282" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B282" s="0" t="s">
+      <c r="B282" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4292,7 +4310,7 @@
       <c r="A283" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B283" s="0" t="s">
+      <c r="B283" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4300,7 +4318,7 @@
       <c r="A284" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B284" s="0" t="s">
+      <c r="B284" s="3" t="s">
         <v>334</v>
       </c>
     </row>
@@ -4308,7 +4326,7 @@
       <c r="A285" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B285" s="0" t="s">
+      <c r="B285" s="3" t="s">
         <v>336</v>
       </c>
     </row>
@@ -4316,7 +4334,7 @@
       <c r="A286" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B286" s="0" t="s">
+      <c r="B286" s="3" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4324,7 +4342,7 @@
       <c r="A287" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B287" s="0" t="s">
+      <c r="B287" s="3" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4332,7 +4350,7 @@
       <c r="A288" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B288" s="0" t="s">
+      <c r="B288" s="3" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4340,7 +4358,7 @@
       <c r="A289" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B289" s="0" t="s">
+      <c r="B289" s="3" t="s">
         <v>339</v>
       </c>
     </row>
@@ -4348,7 +4366,7 @@
       <c r="A290" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B290" s="0" t="s">
+      <c r="B290" s="3" t="s">
         <v>174</v>
       </c>
     </row>
@@ -4356,7 +4374,7 @@
       <c r="A291" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B291" s="0" t="s">
+      <c r="B291" s="3" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4364,7 +4382,7 @@
       <c r="A292" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B292" s="0" t="s">
+      <c r="B292" s="3" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4372,8 +4390,104 @@
       <c r="A293" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B293" s="0" t="s">
+      <c r="B293" s="3" t="s">
         <v>341</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B297" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B298" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B300" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B302" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B305" s="4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4422,25 +4536,25 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="H1" s="11"/>
     </row>
@@ -4448,7 +4562,7 @@
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="14" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="15"/>
@@ -4458,38 +4572,38 @@
     </row>
     <row r="4" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
     </row>
     <row r="5" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
@@ -4505,19 +4619,19 @@
         <v>48</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4530,82 +4644,82 @@
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="17" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="9" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>364</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>358</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
     <row r="10" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="E10" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>358</v>
-      </c>
       <c r="G10" s="16" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>358</v>
-      </c>
       <c r="G11" s="16" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4620,7 +4734,7 @@
     </row>
     <row r="13" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>17</v>
@@ -4629,19 +4743,19 @@
         <v>18</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4649,44 +4763,44 @@
         <v>23</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
     <row r="15" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
     <row r="16" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>11</v>
@@ -4695,20 +4809,20 @@
         <v>67</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
     </row>
     <row r="17" s="19" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>22</v>
@@ -4718,10 +4832,10 @@
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="17" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -4732,25 +4846,25 @@
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="14" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>51</v>
@@ -4758,69 +4872,69 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>395</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>388</v>
-      </c>
       <c r="F23" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H23" s="16"/>
     </row>
     <row r="24" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>59</v>
@@ -4828,10 +4942,10 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
@@ -4845,13 +4959,13 @@
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="24" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
@@ -4866,10 +4980,10 @@
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
@@ -4885,29 +4999,29 @@
         <v>18</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
     <row r="29" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="26"/>
@@ -4916,22 +5030,22 @@
     </row>
     <row r="30" s="19" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
@@ -4948,10 +5062,10 @@
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
@@ -4968,10 +5082,10 @@
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="23" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>

</xml_diff>